<commit_message>
removed N poly in step 4
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1b_CO2_Fluid_Inclusions/FI_fitting.xlsx
+++ b/docs/Examples/Example1b_CO2_Fluid_Inclusions/FI_fitting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="124">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Corr_Split-1σ</t>
+  </si>
+  <si>
+    <t>Corr_Split_1σ_val</t>
   </si>
   <si>
     <t>filename_x</t>
@@ -757,13 +760,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BG17"/>
+  <dimension ref="A1:BH17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:59">
+    <row r="1" spans="1:60">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -938,8 +941,11 @@
       <c r="BG1" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="BH1" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="2" spans="1:59">
+    <row r="2" spans="1:60">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -947,118 +953,121 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>102.8362594207548</v>
+        <v>102.8361615588676</v>
       </c>
       <c r="D2">
-        <v>102.8406405597869</v>
+        <v>102.8405494867341</v>
       </c>
       <c r="E2">
-        <v>102.8318782817228</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2">
+        <v>102.831773631001</v>
+      </c>
+      <c r="F2">
+        <v>0.004387927866552325</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2">
         <v>103.0582462663822</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>1286.035113895083</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.00436</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>592.2737949387184</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1286.035113895083</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>607.8614501662316</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.4337375273315542</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>3.691375804853168</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.3099470578599591</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>0.8674750546631085</v>
       </c>
-      <c r="S2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T2">
+      <c r="T2" t="s">
+        <v>75</v>
+      </c>
+      <c r="U2">
         <v>1389.093360161465</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>968.2088497370656</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>1389.093360161465</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>904.3471417817207</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>0.3954978034139988</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>3.743551243633247</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>0.3078957175034538</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>0.7909956068279975</v>
       </c>
-      <c r="AD2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT2" t="s">
+      <c r="AE2" t="s">
         <v>75</v>
       </c>
       <c r="AU2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AV2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="AW2" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="AX2" t="s">
         <v>104</v>
       </c>
-      <c r="AY2">
+      <c r="AY2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ2">
         <v>28</v>
       </c>
-      <c r="BA2">
+      <c r="BB2">
         <v>45</v>
       </c>
-      <c r="BB2">
+      <c r="BC2">
         <v>5</v>
       </c>
-      <c r="BC2">
+      <c r="BD2">
         <v>50</v>
       </c>
-      <c r="BD2" t="s">
-        <v>105</v>
-      </c>
       <c r="BE2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BF2">
+        <v>106</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BG2">
         <v>43795</v>
       </c>
-      <c r="BG2">
+      <c r="BH2">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="3" spans="1:59">
+    <row r="3" spans="1:60">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1066,127 +1075,130 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>102.7878818311173</v>
+        <v>102.7879155353095</v>
       </c>
       <c r="D3">
-        <v>102.8001029749293</v>
+        <v>102.8001390682454</v>
       </c>
       <c r="E3">
-        <v>102.7756606873052</v>
-      </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3">
+        <v>102.7756920023735</v>
+      </c>
+      <c r="F3">
+        <v>0.01222353293590281</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3">
         <v>103.0106887739485</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.01727</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.01223693180499099</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>1286.157462583564</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.00919</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>227.6699213181409</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1286.157462583564</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>201.585655651332</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.4094465731597128</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>3.372069054466578</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.0414472417507597</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>0.8188931463194256</v>
       </c>
-      <c r="S3" t="s">
-        <v>74</v>
-      </c>
-      <c r="T3">
+      <c r="T3" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3">
         <v>1389.168151357512</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>0.00808</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>374.138446400111</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>1389.168151357512</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>344.0597686324394</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>0.3881542915910066</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>3.622729205113153</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>0.3189631546474725</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>0.7763085831820131</v>
       </c>
-      <c r="AD3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>59</v>
+      <c r="AE3" t="s">
+        <v>75</v>
       </c>
       <c r="AU3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AV3" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="AW3" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="AX3" t="s">
         <v>104</v>
       </c>
-      <c r="AY3">
+      <c r="AY3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ3">
         <v>28</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>45</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <v>5</v>
       </c>
-      <c r="BC3">
+      <c r="BD3">
         <v>50</v>
       </c>
-      <c r="BD3" t="s">
-        <v>105</v>
-      </c>
       <c r="BE3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BF3">
+        <v>106</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>109</v>
+      </c>
+      <c r="BG3">
         <v>44393</v>
       </c>
-      <c r="BG3">
+      <c r="BH3">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:60">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1194,127 +1206,130 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>102.8223777310256</v>
+        <v>102.8225348192964</v>
       </c>
       <c r="D4">
-        <v>102.8284061268009</v>
+        <v>102.8285679468984</v>
       </c>
       <c r="E4">
-        <v>102.8163493352503</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4">
+        <v>102.8165016916945</v>
+      </c>
+      <c r="F4">
+        <v>0.006033127601982144</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4">
         <v>103.0463331604426</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.00848</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.006020298995897131</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1286.07409088711</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.00462</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>570.4088802070202</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1286.07409088711</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>582.2966960566378</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.422212103948058</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>3.767917651067944</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.3700721476420182</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0.8444242078961161</v>
       </c>
-      <c r="S4" t="s">
-        <v>74</v>
-      </c>
-      <c r="T4">
+      <c r="T4" t="s">
+        <v>75</v>
+      </c>
+      <c r="U4">
         <v>1389.120424047552</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>0.00386</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>888.685802695913</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>1389.120424047552</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>839.6197329417737</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>0.3996293378353412</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>3.922465297191736</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>0.3102594975762186</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>0.7992586756706823</v>
       </c>
-      <c r="AD4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>76</v>
+      <c r="AE4" t="s">
+        <v>75</v>
       </c>
       <c r="AU4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AV4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="AW4" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="AX4" t="s">
         <v>104</v>
       </c>
-      <c r="AY4">
+      <c r="AY4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ4">
         <v>28</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <v>45</v>
       </c>
-      <c r="BB4">
+      <c r="BC4">
         <v>5</v>
       </c>
-      <c r="BC4">
+      <c r="BD4">
         <v>50</v>
       </c>
-      <c r="BD4" t="s">
-        <v>105</v>
-      </c>
       <c r="BE4" t="s">
-        <v>109</v>
-      </c>
-      <c r="BF4">
+        <v>106</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>110</v>
+      </c>
+      <c r="BG4">
         <v>45146</v>
       </c>
-      <c r="BG4">
+      <c r="BH4">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="5" spans="1:59">
+    <row r="5" spans="1:60">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1322,127 +1337,130 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>103.0846445570404</v>
+        <v>103.0848863374035</v>
       </c>
       <c r="D5">
-        <v>103.1164915061394</v>
+        <v>103.1167342397108</v>
       </c>
       <c r="E5">
-        <v>103.0527976079414</v>
-      </c>
-      <c r="F5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5">
+        <v>103.0530384350963</v>
+      </c>
+      <c r="F5">
+        <v>0.03184790230725106</v>
+      </c>
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5">
         <v>103.3102060063391</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.0422</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.03191269339933563</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>1285.4319007168</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.0291</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>66.02212482602798</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1285.4319007168</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>82.0817529134724</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.5784420090217476</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>3.130955921886279</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>1.160394290100619E-07</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>1.156884018043495</v>
       </c>
-      <c r="S5" t="s">
-        <v>74</v>
-      </c>
-      <c r="T5">
+      <c r="T5" t="s">
+        <v>75</v>
+      </c>
+      <c r="U5">
         <v>1388.742106723139</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>0.0131</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>129.4479100528684</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>1388.742106723139</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>167.5656015298983</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>0.4790586259665257</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>2.390976621497358</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>0.6659269750496657</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>0.9581172519330513</v>
       </c>
-      <c r="AD5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>77</v>
+      <c r="AE5" t="s">
+        <v>75</v>
       </c>
       <c r="AU5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AV5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AW5" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="AX5" t="s">
         <v>104</v>
       </c>
-      <c r="AY5">
+      <c r="AY5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ5">
         <v>28</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>45</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <v>5</v>
       </c>
-      <c r="BC5">
+      <c r="BD5">
         <v>50</v>
       </c>
-      <c r="BD5" t="s">
-        <v>105</v>
-      </c>
       <c r="BE5" t="s">
-        <v>110</v>
-      </c>
-      <c r="BF5">
+        <v>106</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>111</v>
+      </c>
+      <c r="BG5">
         <v>45944</v>
       </c>
-      <c r="BG5">
+      <c r="BH5">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:60">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1450,127 +1468,130 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>103.0787002551172</v>
+        <v>103.0789625307259</v>
       </c>
       <c r="D6">
-        <v>103.0831613947997</v>
+        <v>103.0834298983843</v>
       </c>
       <c r="E6">
-        <v>103.0742391154346</v>
-      </c>
-      <c r="F6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6">
+        <v>103.0744951630676</v>
+      </c>
+      <c r="F6">
+        <v>0.004467367658349187</v>
+      </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6">
         <v>103.3046141292737</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.00626</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.00444292696316291</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1285.4357628688</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.00286</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>607.8099966205095</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1285.4357628688</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>895.852963265536</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.5682515482486674</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>3.891747696659221</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>0.5562907908348357</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>1.136503096497335</v>
       </c>
-      <c r="S6" t="s">
-        <v>74</v>
-      </c>
-      <c r="T6">
+      <c r="T6" t="s">
+        <v>75</v>
+      </c>
+      <c r="U6">
         <v>1388.740376998074</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>0.0034</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>1147.746938022313</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>1388.740376998074</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>1426.205783795498</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>0.4810902865979522</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>4.05606289695736</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>0.5486864959122263</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>0.9621805731959044</v>
       </c>
-      <c r="AD6" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>78</v>
+      <c r="AE6" t="s">
+        <v>75</v>
       </c>
       <c r="AU6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AV6" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AW6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AX6" t="s">
         <v>104</v>
       </c>
-      <c r="AY6">
+      <c r="AY6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ6">
         <v>28</v>
       </c>
-      <c r="BA6">
+      <c r="BB6">
         <v>45</v>
       </c>
-      <c r="BB6">
+      <c r="BC6">
         <v>5</v>
       </c>
-      <c r="BC6">
+      <c r="BD6">
         <v>50</v>
       </c>
-      <c r="BD6" t="s">
-        <v>106</v>
-      </c>
       <c r="BE6" t="s">
-        <v>111</v>
-      </c>
-      <c r="BF6">
+        <v>107</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>112</v>
+      </c>
+      <c r="BG6">
         <v>46247</v>
       </c>
-      <c r="BG6">
+      <c r="BH6">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="7" spans="1:59">
+    <row r="7" spans="1:60">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1578,127 +1599,130 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>103.1107801775993</v>
+        <v>103.1107229183252</v>
       </c>
       <c r="D7">
-        <v>103.1228892612657</v>
+        <v>103.1228341394692</v>
       </c>
       <c r="E7">
-        <v>103.0986710939329</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7">
+        <v>103.0986116971812</v>
+      </c>
+      <c r="F7">
+        <v>0.01211122114400514</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7">
         <v>103.3410502964659</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.01649</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.01212650403042856</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1285.310758066639</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.0106</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>125.5499417899416</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>1285.310758066639</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>210.7357317789604</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0.6314606662445564</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>1.840530773602764</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>0.6219953983111839</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>1.262921332489113</v>
       </c>
-      <c r="S7" t="s">
-        <v>74</v>
-      </c>
-      <c r="T7">
+      <c r="T7" t="s">
+        <v>75</v>
+      </c>
+      <c r="U7">
         <v>1388.651808363104</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>0.00589</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>235.75108839194</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>1388.651808363104</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>317.853774041187</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>0.5313379863731259</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>1.767705384929408</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>0.505521083901327</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>1.062675972746252</v>
       </c>
-      <c r="AD7" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>79</v>
+      <c r="AE7" t="s">
+        <v>75</v>
       </c>
       <c r="AU7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AV7" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AW7" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="AX7" t="s">
         <v>104</v>
       </c>
-      <c r="AY7">
+      <c r="AY7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ7">
         <v>28</v>
       </c>
-      <c r="BA7">
+      <c r="BB7">
         <v>45</v>
       </c>
-      <c r="BB7">
+      <c r="BC7">
         <v>5</v>
       </c>
-      <c r="BC7">
+      <c r="BD7">
         <v>50</v>
       </c>
-      <c r="BD7" t="s">
-        <v>106</v>
-      </c>
       <c r="BE7" t="s">
-        <v>112</v>
-      </c>
-      <c r="BF7">
+        <v>107</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>113</v>
+      </c>
+      <c r="BG7">
         <v>51532</v>
       </c>
-      <c r="BG7">
+      <c r="BH7">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="8" spans="1:59">
+    <row r="8" spans="1:60">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1706,127 +1730,130 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>103.0702520787559</v>
+        <v>103.0700212561137</v>
       </c>
       <c r="D8">
-        <v>103.0759324437156</v>
+        <v>103.0757062037854</v>
       </c>
       <c r="E8">
-        <v>103.0645717137963</v>
-      </c>
-      <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8">
+        <v>103.064336308442</v>
+      </c>
+      <c r="F8">
+        <v>0.005684947671667892</v>
+      </c>
+      <c r="G8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8">
         <v>103.3010011193155</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.007980000000000001</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.005672424525720902</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1285.407637048017</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>0.0044</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>519.6084806096436</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>1285.407637048017</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>812.182813229279</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.5633759888840726</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>3.854109522307193</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>0.7243914854037556</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>1.126751977768145</v>
       </c>
-      <c r="S8" t="s">
-        <v>74</v>
-      </c>
-      <c r="T8">
+      <c r="T8" t="s">
+        <v>75</v>
+      </c>
+      <c r="U8">
         <v>1388.708638167333</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>0.00358</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>938.3906823007294</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>1388.708638167333</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>1219.110015942939</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>0.5075643715207541</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>3.674296521167622</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <v>0.5250339636234796</v>
       </c>
-      <c r="AC8">
+      <c r="AD8">
         <v>1.015128743041508</v>
       </c>
-      <c r="AD8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>80</v>
+      <c r="AE8" t="s">
+        <v>75</v>
       </c>
       <c r="AU8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AV8" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="AW8" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="AX8" t="s">
         <v>104</v>
       </c>
-      <c r="AY8">
+      <c r="AY8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ8">
         <v>28</v>
       </c>
-      <c r="BA8">
+      <c r="BB8">
         <v>45</v>
       </c>
-      <c r="BB8">
+      <c r="BC8">
         <v>5</v>
       </c>
-      <c r="BC8">
+      <c r="BD8">
         <v>50</v>
       </c>
-      <c r="BD8" t="s">
-        <v>106</v>
-      </c>
       <c r="BE8" t="s">
-        <v>113</v>
-      </c>
-      <c r="BF8">
+        <v>107</v>
+      </c>
+      <c r="BF8" t="s">
+        <v>114</v>
+      </c>
+      <c r="BG8">
         <v>52872</v>
       </c>
-      <c r="BG8">
+      <c r="BH8">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="9" spans="1:59">
+    <row r="9" spans="1:60">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1834,127 +1861,130 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>103.0571279116327</v>
+        <v>103.0572682304521</v>
       </c>
       <c r="D9">
-        <v>103.0667036915539</v>
+        <v>103.0668475017843</v>
       </c>
       <c r="E9">
-        <v>103.0475521317116</v>
-      </c>
-      <c r="F9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9">
+        <v>103.04768895912</v>
+      </c>
+      <c r="F9">
+        <v>0.009579271332130464</v>
+      </c>
+      <c r="G9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9">
         <v>103.2888796361788</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.01323</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.009581696092028802</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1285.392842722296</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.00808</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>158.6481192449043</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1285.392842722296</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>249.5983531706096</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>0.6197349920296515</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>1.485895460054742</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>0.5025194426469294</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>1.239469984059303</v>
       </c>
-      <c r="S9" t="s">
-        <v>74</v>
-      </c>
-      <c r="T9">
+      <c r="T9" t="s">
+        <v>75</v>
+      </c>
+      <c r="U9">
         <v>1388.681722358475</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>0.00515</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>296.1306896936336</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>1388.681722358475</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>390.8443640991435</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>0.5144726769650321</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>1.934053961295279</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>0.531608288309546</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <v>1.028945353930064</v>
       </c>
-      <c r="AD9" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>81</v>
+      <c r="AE9" t="s">
+        <v>75</v>
       </c>
       <c r="AU9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AV9" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="AW9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="AX9" t="s">
         <v>104</v>
       </c>
-      <c r="AY9">
+      <c r="AY9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ9">
         <v>28</v>
       </c>
-      <c r="BA9">
+      <c r="BB9">
         <v>45</v>
       </c>
-      <c r="BB9">
+      <c r="BC9">
         <v>5</v>
       </c>
-      <c r="BC9">
+      <c r="BD9">
         <v>50</v>
       </c>
-      <c r="BD9" t="s">
-        <v>106</v>
-      </c>
       <c r="BE9" t="s">
-        <v>114</v>
-      </c>
-      <c r="BF9">
+        <v>107</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>115</v>
+      </c>
+      <c r="BG9">
         <v>61553</v>
       </c>
-      <c r="BG9">
+      <c r="BH9">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="10" spans="1:59">
+    <row r="10" spans="1:60">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1962,154 +1992,157 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>103.0730670006625</v>
+        <v>103.0733568833525</v>
       </c>
       <c r="D10">
-        <v>103.0752099354824</v>
+        <v>103.0755124222568</v>
       </c>
       <c r="E10">
-        <v>103.0709240658427</v>
-      </c>
-      <c r="F10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10">
+        <v>103.0712013444481</v>
+      </c>
+      <c r="F10">
+        <v>0.002155538904362311</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10">
         <v>103.3001275115473</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.00284</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.002090215299915298</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1285.470024218834</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0.00183</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>988.9447625563595</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>1285.470074221334</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>1433.106729155515</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>0.5526607383916854</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>2.918337425880185</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>0.583487251346276</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>1.105321476783371</v>
       </c>
-      <c r="S10" t="s">
-        <v>74</v>
-      </c>
-      <c r="T10">
+      <c r="T10" t="s">
+        <v>75</v>
+      </c>
+      <c r="U10">
         <v>1388.770251735381</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>0.00101</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>1865.050087900247</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>1388.770201732881</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>2295.957876844293</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>0.4800414907782372</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>2.981931218669617</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <v>0.5270224678879835</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>0.9600829815564743</v>
       </c>
-      <c r="AD10" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE10">
+      <c r="AE10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF10">
         <v>1265.20238248543</v>
       </c>
-      <c r="AF10">
+      <c r="AG10">
         <v>102.3323757836743</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <v>0.801804627174481</v>
       </c>
-      <c r="AH10">
+      <c r="AI10">
         <v>1410.117692412663</v>
       </c>
-      <c r="AI10">
+      <c r="AJ10">
         <v>255.6139528573827</v>
       </c>
-      <c r="AJ10">
+      <c r="AK10">
         <v>0.6082758618519937</v>
       </c>
-      <c r="AK10">
+      <c r="AL10">
         <v>1371.200733191896</v>
       </c>
-      <c r="AL10">
+      <c r="AM10">
         <v>24.95844077179569</v>
       </c>
-      <c r="AM10">
+      <c r="AN10">
         <v>0.2396594143607584</v>
       </c>
-      <c r="AT10" t="s">
-        <v>66</v>
-      </c>
       <c r="AU10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AV10" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="AW10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="AX10" t="s">
         <v>104</v>
       </c>
-      <c r="AY10">
+      <c r="AY10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ10">
         <v>28</v>
       </c>
-      <c r="BA10">
+      <c r="BB10">
         <v>45</v>
       </c>
-      <c r="BB10">
+      <c r="BC10">
         <v>5</v>
       </c>
-      <c r="BC10">
+      <c r="BD10">
         <v>50</v>
       </c>
-      <c r="BD10" t="s">
-        <v>106</v>
-      </c>
       <c r="BE10" t="s">
-        <v>115</v>
-      </c>
-      <c r="BF10">
+        <v>107</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>116</v>
+      </c>
+      <c r="BG10">
         <v>47301</v>
       </c>
-      <c r="BG10">
+      <c r="BH10">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="11" spans="1:59">
+    <row r="11" spans="1:60">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2117,154 +2150,157 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>103.1056120804964</v>
+        <v>103.1058669070527</v>
       </c>
       <c r="D11">
-        <v>103.1078284418133</v>
+        <v>103.1080952171408</v>
       </c>
       <c r="E11">
-        <v>103.1033957191796</v>
-      </c>
-      <c r="F11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11">
+        <v>103.1036385969647</v>
+      </c>
+      <c r="F11">
+        <v>0.00222831008802797</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11">
         <v>103.3338108167045</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.00302</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.002166887168266959</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1285.409241156897</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>0.00177</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>815.5836622657513</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>1285.409291159397</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>1225.330166596846</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>0.556970575662959</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>2.339882688767294</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>0.6539945627595156</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>1.113941151325918</v>
       </c>
-      <c r="S11" t="s">
-        <v>74</v>
-      </c>
-      <c r="T11">
+      <c r="T11" t="s">
+        <v>75</v>
+      </c>
+      <c r="U11">
         <v>1388.743151978602</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>0.00125</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>1535.09123885693</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>1388.743101976102</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>1950.409825502654</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>0.4920361949202328</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>2.704154294701641</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>0.5447818793539625</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>0.9840723898404655</v>
       </c>
-      <c r="AD11" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE11">
+      <c r="AE11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF11">
         <v>1265.24176447645</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <v>101.2476738290779</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <v>0.7463094195392324</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <v>1410.07744109423</v>
       </c>
-      <c r="AI11">
+      <c r="AJ11">
         <v>223.3562026881224</v>
       </c>
-      <c r="AJ11">
+      <c r="AK11">
         <v>0.6875935622364313</v>
       </c>
-      <c r="AK11">
+      <c r="AL11">
         <v>1370.363006784529</v>
       </c>
-      <c r="AL11">
+      <c r="AM11">
         <v>25.23506880600382</v>
       </c>
-      <c r="AM11">
+      <c r="AN11">
         <v>0.2457192656728297</v>
       </c>
-      <c r="AT11" t="s">
-        <v>67</v>
-      </c>
       <c r="AU11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AV11" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="AW11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="AX11" t="s">
         <v>104</v>
       </c>
-      <c r="AY11">
+      <c r="AY11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ11">
         <v>28</v>
       </c>
-      <c r="BA11">
+      <c r="BB11">
         <v>45</v>
       </c>
-      <c r="BB11">
+      <c r="BC11">
         <v>5</v>
       </c>
-      <c r="BC11">
+      <c r="BD11">
         <v>50</v>
       </c>
-      <c r="BD11" t="s">
-        <v>105</v>
-      </c>
       <c r="BE11" t="s">
-        <v>116</v>
-      </c>
-      <c r="BF11">
+        <v>106</v>
+      </c>
+      <c r="BF11" t="s">
+        <v>117</v>
+      </c>
+      <c r="BG11">
         <v>48438</v>
       </c>
-      <c r="BG11">
+      <c r="BH11">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="12" spans="1:59">
+    <row r="12" spans="1:60">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2272,154 +2308,157 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>103.0762596975463</v>
+        <v>103.0760612138406</v>
       </c>
       <c r="D12">
-        <v>103.0797873867596</v>
+        <v>103.0795962776327</v>
       </c>
       <c r="E12">
-        <v>103.072732008333</v>
-      </c>
-      <c r="F12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12">
+        <v>103.0725261500485</v>
+      </c>
+      <c r="F12">
+        <v>0.003535063792098491</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12">
         <v>103.3069278981677</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.00454</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.003502284968417048</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>1285.401620260415</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.00326</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>894.5760598357432</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>1285.401670262915</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>1408.035216662493</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.5873074890845776</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>2.73028985885123</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>0.6379960730781123</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>1.174614978169155</v>
       </c>
-      <c r="S12" t="s">
-        <v>74</v>
-      </c>
-      <c r="T12">
+      <c r="T12" t="s">
+        <v>75</v>
+      </c>
+      <c r="U12">
         <v>1388.708648163583</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>0.00128</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>1646.280180725079</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>1388.708598161083</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>2156.307344215023</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>0.5043365654601331</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>2.570167096328094</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>0.5593802263665194</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>1.008673130920266</v>
       </c>
-      <c r="AD12" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE12">
+      <c r="AE12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF12">
         <v>1265.117868946772</v>
       </c>
-      <c r="AF12">
+      <c r="AG12">
         <v>118.4877711345881</v>
       </c>
-      <c r="AG12">
+      <c r="AH12">
         <v>0.8950807458652681</v>
       </c>
-      <c r="AH12">
+      <c r="AI12">
         <v>1410.029892389665</v>
       </c>
-      <c r="AI12">
+      <c r="AJ12">
         <v>240.5008031753221</v>
       </c>
-      <c r="AJ12">
+      <c r="AK12">
         <v>0.6510665975504503</v>
       </c>
-      <c r="AK12">
+      <c r="AL12">
         <v>1370.599368698509</v>
       </c>
-      <c r="AL12">
+      <c r="AM12">
         <v>29.96538600911319</v>
       </c>
-      <c r="AM12">
+      <c r="AN12">
         <v>0.2519697882420668</v>
       </c>
-      <c r="AT12" t="s">
-        <v>82</v>
-      </c>
       <c r="AU12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AV12" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="AW12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="AX12" t="s">
         <v>104</v>
       </c>
-      <c r="AY12">
+      <c r="AY12" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ12">
         <v>28</v>
       </c>
-      <c r="BA12">
+      <c r="BB12">
         <v>45</v>
       </c>
-      <c r="BB12">
+      <c r="BC12">
         <v>5</v>
       </c>
-      <c r="BC12">
+      <c r="BD12">
         <v>50</v>
       </c>
-      <c r="BD12" t="s">
-        <v>106</v>
-      </c>
       <c r="BE12" t="s">
-        <v>117</v>
-      </c>
-      <c r="BF12">
+        <v>107</v>
+      </c>
+      <c r="BF12" t="s">
+        <v>118</v>
+      </c>
+      <c r="BG12">
         <v>52620</v>
       </c>
-      <c r="BG12">
+      <c r="BH12">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="13" spans="1:59">
+    <row r="13" spans="1:60">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2427,145 +2466,148 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>103.0700692721945</v>
+        <v>103.0697563007783</v>
       </c>
       <c r="D13">
-        <v>103.0712510078531</v>
+        <v>103.0709600746594</v>
       </c>
       <c r="E13">
-        <v>103.0688875365359</v>
-      </c>
-      <c r="F13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13">
+        <v>103.0685525268972</v>
+      </c>
+      <c r="F13">
+        <v>0.001203773881074386</v>
+      </c>
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13">
         <v>103.3010395221575</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>1285.380950644217</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>1350.098658951685</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>1285.381000646717</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>2155.05514656322</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>0.5861968908412568</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>2.606137731588801</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>0.6770671704029785</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>1.172393781682514</v>
       </c>
-      <c r="S13" t="s">
-        <v>74</v>
-      </c>
-      <c r="T13">
+      <c r="T13" t="s">
+        <v>75</v>
+      </c>
+      <c r="U13">
         <v>1388.682090171375</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>0.00108</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>2473.763433395881</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>1388.682040168875</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>3286.543283427551</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>0.5132277110661194</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>3.342951449103059</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <v>0.5510920683940045</v>
       </c>
-      <c r="AC13">
+      <c r="AD13">
         <v>1.026455422132239</v>
       </c>
-      <c r="AD13" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE13">
+      <c r="AE13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF13">
         <v>1265.141741547915</v>
       </c>
-      <c r="AF13">
+      <c r="AG13">
         <v>225.1357170601105</v>
       </c>
-      <c r="AG13">
+      <c r="AH13">
         <v>0.753521738703524</v>
       </c>
-      <c r="AH13">
+      <c r="AI13">
         <v>1410.023726704886</v>
       </c>
-      <c r="AI13">
+      <c r="AJ13">
         <v>359.972150413653</v>
       </c>
-      <c r="AJ13">
+      <c r="AK13">
         <v>0.6528277779392482</v>
       </c>
-      <c r="AK13">
+      <c r="AL13">
         <v>1370.31245887703</v>
       </c>
-      <c r="AL13">
+      <c r="AM13">
         <v>47.48535288301242</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <v>0.2564642403779516</v>
       </c>
-      <c r="AT13" t="s">
-        <v>83</v>
-      </c>
       <c r="AU13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AV13" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="AW13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="AX13" t="s">
         <v>104</v>
       </c>
-      <c r="AY13">
+      <c r="AY13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ13">
         <v>28</v>
       </c>
-      <c r="BA13">
+      <c r="BB13">
         <v>45</v>
       </c>
-      <c r="BB13">
+      <c r="BC13">
         <v>5</v>
       </c>
-      <c r="BC13">
+      <c r="BD13">
         <v>50</v>
       </c>
-      <c r="BD13" t="s">
-        <v>106</v>
-      </c>
       <c r="BE13" t="s">
-        <v>118</v>
-      </c>
-      <c r="BF13">
+        <v>107</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>119</v>
+      </c>
+      <c r="BG13">
         <v>53534</v>
       </c>
-      <c r="BG13">
+      <c r="BH13">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="14" spans="1:59">
+    <row r="14" spans="1:60">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2573,154 +2615,157 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>103.0215226197999</v>
+        <v>103.0211727340567</v>
       </c>
       <c r="D14">
-        <v>103.023259490921</v>
+        <v>103.0229247168622</v>
       </c>
       <c r="E14">
-        <v>103.0197857486787</v>
-      </c>
-      <c r="F14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14">
+        <v>103.0194207512512</v>
+      </c>
+      <c r="F14">
+        <v>0.00175198280551737</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14">
         <v>103.25247720026</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.002237</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.001671277654969395</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>1285.586972031724</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.0015</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>858.6196462984607</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>1285.587022034224</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>1179.510115201747</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>0.5310479220429358</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>1.997212682716575</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>0.5493171500494235</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>1.062095844085872</v>
       </c>
-      <c r="S14" t="s">
-        <v>74</v>
-      </c>
-      <c r="T14">
+      <c r="T14" t="s">
+        <v>75</v>
+      </c>
+      <c r="U14">
         <v>1388.839549236985</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>0.000737</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>1547.88806296731</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>1388.839499234484</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>1820.132849326528</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>0.46058840286098</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>2.048995397492688</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <v>0.515420564601423</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>0.9211768057219599</v>
       </c>
-      <c r="AD14" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE14">
+      <c r="AE14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF14">
         <v>1265.336600548907</v>
       </c>
-      <c r="AF14">
+      <c r="AG14">
         <v>128.6834076152618</v>
       </c>
-      <c r="AG14">
+      <c r="AH14">
         <v>0.7151000742016528</v>
       </c>
-      <c r="AH14">
+      <c r="AI14">
         <v>1410.145385844362</v>
       </c>
-      <c r="AI14">
+      <c r="AJ14">
         <v>203.1236646688626</v>
       </c>
-      <c r="AJ14">
+      <c r="AK14">
         <v>0.6080352018977694</v>
       </c>
-      <c r="AK14">
+      <c r="AL14">
         <v>1370.367824436326</v>
       </c>
-      <c r="AL14">
+      <c r="AM14">
         <v>19.13738958356594</v>
       </c>
-      <c r="AM14">
+      <c r="AN14">
         <v>0.2297923549731922</v>
       </c>
-      <c r="AT14" t="s">
-        <v>70</v>
-      </c>
       <c r="AU14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AV14" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="AW14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AX14" t="s">
         <v>104</v>
       </c>
-      <c r="AY14">
+      <c r="AY14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ14">
         <v>28</v>
       </c>
-      <c r="BA14">
+      <c r="BB14">
         <v>45</v>
       </c>
-      <c r="BB14">
+      <c r="BC14">
         <v>5</v>
       </c>
-      <c r="BC14">
+      <c r="BD14">
         <v>50</v>
       </c>
-      <c r="BD14" t="s">
-        <v>106</v>
-      </c>
       <c r="BE14" t="s">
-        <v>119</v>
-      </c>
-      <c r="BF14">
+        <v>107</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>120</v>
+      </c>
+      <c r="BG14">
         <v>53850</v>
       </c>
-      <c r="BG14">
+      <c r="BH14">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="15" spans="1:59">
+    <row r="15" spans="1:60">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2728,145 +2773,148 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>103.0742532121182</v>
+        <v>103.074121484731</v>
       </c>
       <c r="D15">
-        <v>103.0756382510179</v>
+        <v>103.075529504623</v>
       </c>
       <c r="E15">
-        <v>103.0728681732184</v>
-      </c>
-      <c r="F15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15">
+        <v>103.0727134648389</v>
+      </c>
+      <c r="F15">
+        <v>0.001408019892020299</v>
+      </c>
+      <c r="G15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15">
         <v>103.3060348593001</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>1285.373767647719</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>997.8808322152316</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>1285.373817650219</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>1565.900510199585</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>0.5908745790041018</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>3.178118101655344</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>0.6155469047754594</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>1.181749158008204</v>
       </c>
-      <c r="S15" t="s">
-        <v>74</v>
-      </c>
-      <c r="T15">
+      <c r="T15" t="s">
+        <v>75</v>
+      </c>
+      <c r="U15">
         <v>1388.679902512019</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>0.00128</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>1878.068314673153</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>1388.679852509519</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>2486.955780978396</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>0.5128371503402582</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <v>2.809103562500914</v>
       </c>
-      <c r="AB15">
+      <c r="AC15">
         <v>0.5446571324604389</v>
       </c>
-      <c r="AC15">
+      <c r="AD15">
         <v>1.025674300680516</v>
       </c>
-      <c r="AD15" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE15">
+      <c r="AE15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF15">
         <v>1265.109716454702</v>
       </c>
-      <c r="AF15">
+      <c r="AG15">
         <v>140.0725966249752</v>
       </c>
-      <c r="AG15">
+      <c r="AH15">
         <v>0.8505464434302338</v>
       </c>
-      <c r="AH15">
+      <c r="AI15">
         <v>1410.009248213728</v>
       </c>
-      <c r="AI15">
+      <c r="AJ15">
         <v>275.7112639468004</v>
       </c>
-      <c r="AJ15">
+      <c r="AK15">
         <v>0.6729725436533109</v>
       </c>
-      <c r="AK15">
+      <c r="AL15">
         <v>1370.322317635334</v>
       </c>
-      <c r="AL15">
+      <c r="AM15">
         <v>34.08628983793483</v>
       </c>
-      <c r="AM15">
+      <c r="AN15">
         <v>0.2562726557539015</v>
       </c>
-      <c r="AT15" t="s">
-        <v>84</v>
-      </c>
       <c r="AU15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AV15" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="AW15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AX15" t="s">
         <v>104</v>
       </c>
-      <c r="AY15">
+      <c r="AY15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ15">
         <v>28</v>
       </c>
-      <c r="BA15">
+      <c r="BB15">
         <v>45</v>
       </c>
-      <c r="BB15">
+      <c r="BC15">
         <v>5</v>
       </c>
-      <c r="BC15">
+      <c r="BD15">
         <v>50</v>
       </c>
-      <c r="BD15" t="s">
-        <v>106</v>
-      </c>
       <c r="BE15" t="s">
-        <v>120</v>
-      </c>
-      <c r="BF15">
+        <v>107</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>121</v>
+      </c>
+      <c r="BG15">
         <v>60661</v>
       </c>
-      <c r="BG15">
+      <c r="BH15">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="16" spans="1:59">
+    <row r="16" spans="1:60">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2874,145 +2922,148 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>103.0714987023071</v>
+        <v>103.0714475853547</v>
       </c>
       <c r="D16">
-        <v>103.0741971791858</v>
+        <v>103.0741580722306</v>
       </c>
       <c r="E16">
-        <v>103.0688002254283</v>
-      </c>
-      <c r="F16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16">
+        <v>103.0687370984789</v>
+      </c>
+      <c r="F16">
+        <v>0.002710486875884144</v>
+      </c>
+      <c r="G16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16">
         <v>103.3032768640026</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>1285.362566452665</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>0.00265</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>741.9066878607193</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>1285.362616455165</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>1177.881031413747</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>0.593382651329598</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>2.54862684359876</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>0.63388304386915</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>1.186765302659196</v>
       </c>
-      <c r="S16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T16">
+      <c r="T16" t="s">
+        <v>75</v>
+      </c>
+      <c r="U16">
         <v>1388.665943321668</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>1383.795315118154</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>1388.665893319167</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>1829.184776978153</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>0.5145584299508608</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <v>2.618030256133117</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>0.5315099424371011</v>
       </c>
-      <c r="AC16">
+      <c r="AD16">
         <v>1.029116859901722</v>
       </c>
-      <c r="AD16" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE16">
+      <c r="AE16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF16">
         <v>1265.039231718528</v>
       </c>
-      <c r="AF16">
+      <c r="AG16">
         <v>81.4714294092857</v>
       </c>
-      <c r="AG16">
+      <c r="AH16">
         <v>0.7489749616648999</v>
       </c>
-      <c r="AH16">
+      <c r="AI16">
         <v>1410.003405028286</v>
       </c>
-      <c r="AI16">
+      <c r="AJ16">
         <v>199.36272342866</v>
       </c>
-      <c r="AJ16">
+      <c r="AK16">
         <v>0.7052607935304686</v>
       </c>
-      <c r="AK16">
+      <c r="AL16">
         <v>1371.225501161512</v>
       </c>
-      <c r="AL16">
+      <c r="AM16">
         <v>14.8580798362567</v>
       </c>
-      <c r="AM16">
+      <c r="AN16">
         <v>0.2571747779060946</v>
       </c>
-      <c r="AT16" t="s">
-        <v>85</v>
-      </c>
       <c r="AU16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AV16" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="AW16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AX16" t="s">
         <v>104</v>
       </c>
-      <c r="AY16">
+      <c r="AY16" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ16">
         <v>28</v>
       </c>
-      <c r="BA16">
+      <c r="BB16">
         <v>45</v>
       </c>
-      <c r="BB16">
+      <c r="BC16">
         <v>5</v>
       </c>
-      <c r="BC16">
+      <c r="BD16">
         <v>50</v>
       </c>
-      <c r="BD16" t="s">
-        <v>106</v>
-      </c>
       <c r="BE16" t="s">
-        <v>121</v>
-      </c>
-      <c r="BF16">
+        <v>107</v>
+      </c>
+      <c r="BF16" t="s">
+        <v>122</v>
+      </c>
+      <c r="BG16">
         <v>60953</v>
       </c>
-      <c r="BG16">
+      <c r="BH16">
         <v>1325.004</v>
       </c>
     </row>
-    <row r="17" spans="1:59">
+    <row r="17" spans="1:60">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3020,112 +3071,112 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>103.0759530277015</v>
+        <v>103.0759871591487</v>
       </c>
       <c r="D17">
-        <v>103.0781463829044</v>
+        <v>103.0781954521847</v>
       </c>
       <c r="E17">
-        <v>103.0737596724986</v>
-      </c>
-      <c r="F17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17">
+        <v>103.0737788661127</v>
+      </c>
+      <c r="F17">
+        <v>0.002208293036020667</v>
+      </c>
+      <c r="G17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17">
         <v>103.3077438140626</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>1285.341648895762</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>0.00213</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>1184.562521224834</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>1285.341698898262</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>1945.245170559057</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>0.6050020040692057</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>2.982807765110913</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>0.6693574783750242</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>1.210004008138411</v>
       </c>
-      <c r="S17" t="s">
-        <v>74</v>
-      </c>
-      <c r="T17">
+      <c r="T17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U17">
         <v>1388.649492714825</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>2189.849117685088</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>1388.649442712325</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <v>2924.712455560641</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>0.5114140990811215</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <v>3.557065201373308</v>
       </c>
-      <c r="AB17">
+      <c r="AC17">
         <v>0.5734938485577813</v>
       </c>
-      <c r="AC17">
+      <c r="AD17">
         <v>1.022828198162243</v>
       </c>
-      <c r="AD17" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE17">
+      <c r="AE17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF17">
         <v>1265.10104699577</v>
       </c>
-      <c r="AF17">
+      <c r="AG17">
         <v>219.4993388964008</v>
       </c>
-      <c r="AG17">
+      <c r="AH17">
         <v>0.8615792401831359</v>
       </c>
-      <c r="AH17">
+      <c r="AI17">
         <v>1410.009817470318</v>
       </c>
-      <c r="AI17">
+      <c r="AJ17">
         <v>342.6000059785636</v>
       </c>
-      <c r="AJ17">
+      <c r="AK17">
         <v>0.6646875034346202</v>
       </c>
-      <c r="AK17">
+      <c r="AL17">
         <v>1370.298544120003</v>
       </c>
-      <c r="AL17">
+      <c r="AM17">
         <v>42.06859430400307</v>
       </c>
-      <c r="AM17">
+      <c r="AN17">
         <v>0.2555933991687717</v>
       </c>
-      <c r="AT17" t="s">
-        <v>86</v>
-      </c>
       <c r="AU17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AV17" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="AW17" t="s">
         <v>103</v>
@@ -3133,28 +3184,31 @@
       <c r="AX17" t="s">
         <v>104</v>
       </c>
-      <c r="AY17">
+      <c r="AY17" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ17">
         <v>28</v>
       </c>
-      <c r="BA17">
+      <c r="BB17">
         <v>45</v>
       </c>
-      <c r="BB17">
+      <c r="BC17">
         <v>5</v>
       </c>
-      <c r="BC17">
+      <c r="BD17">
         <v>50</v>
       </c>
-      <c r="BD17" t="s">
-        <v>106</v>
-      </c>
       <c r="BE17" t="s">
-        <v>122</v>
-      </c>
-      <c r="BF17">
+        <v>107</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>123</v>
+      </c>
+      <c r="BG17">
         <v>61234</v>
       </c>
-      <c r="BG17">
+      <c r="BH17">
         <v>1325.004</v>
       </c>
     </row>

</xml_diff>